<commit_message>
Version stable - Generation STF par STF sur premiere feuille du stf template
</commit_message>
<xml_diff>
--- a/mdm/STFG_MDA.xlsx
+++ b/mdm/STFG_MDA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\Scripts\STF_Generator\mdm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31842D49-9820-4CEC-A8BA-5F9FE0028DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4F59EF-C1F3-41A7-9C4B-8F6AEDBDF4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="63">
   <si>
     <t>ElemSys</t>
   </si>
@@ -84,9 +84,6 @@
   </si>
   <si>
     <t>LINE REVISION</t>
-  </si>
-  <si>
-    <t>Field label</t>
   </si>
   <si>
     <t>Actuator</t>
@@ -381,7 +378,7 @@
   </sortState>
   <tableColumns count="9">
     <tableColumn id="11" xr3:uid="{F24956A3-9E2B-4F15-AFA3-93301E00FAA9}" name="Order"/>
-    <tableColumn id="2" xr3:uid="{7C9D3502-DEAA-4E6A-AD5C-9B9B3E25D96E}" name="Field label"/>
+    <tableColumn id="2" xr3:uid="{7C9D3502-DEAA-4E6A-AD5C-9B9B3E25D96E}" name="Label"/>
     <tableColumn id="3" xr3:uid="{B003E680-8671-4B35-8B82-FDCA104FEDEE}" name="Facet"/>
     <tableColumn id="8" xr3:uid="{C4DE5643-8B5D-4C68-8E91-CA3097D11F26}" name="Parent Object"/>
     <tableColumn id="4" xr3:uid="{5F1CC26A-F85C-4D9E-958B-626AAEE5C81E}" name="MUDU"/>
@@ -691,7 +688,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,31 +705,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="G1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -743,25 +740,25 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -772,25 +769,25 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -798,28 +795,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
         <v>62</v>
       </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>63</v>
-      </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -827,28 +824,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -859,25 +856,25 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -888,25 +885,25 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -917,25 +914,25 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E8" t="s">
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -943,28 +940,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" t="s">
         <v>44</v>
       </c>
-      <c r="C9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" t="s">
         <v>45</v>
       </c>
-      <c r="F9" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" t="s">
-        <v>46</v>
-      </c>
       <c r="I9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -975,25 +972,25 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1001,28 +998,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1030,28 +1027,28 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1059,28 +1056,28 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1088,28 +1085,28 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1120,25 +1117,25 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
         <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1146,28 +1143,28 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1195,47 +1192,47 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1263,34 +1260,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
         <v>53</v>
-      </c>
-      <c r="B1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MaJ stable: retrait bar de progression et fix du bouton export STF seul
</commit_message>
<xml_diff>
--- a/mdm/STFG_MDA.xlsx
+++ b/mdm/STFG_MDA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Desktop\Scripts\STF_Generator\mdm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB0B68D-2360-4713-ABCC-1D2B152E6491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5893F804-6ED7-453F-ACC2-FECD56AA4AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="70">
   <si>
     <t>ElemSys</t>
   </si>
@@ -128,15 +128,9 @@
     <t>ValvFailSfPositn</t>
   </si>
   <si>
-    <t>Actuator;Sensor</t>
-  </si>
-  <si>
     <t>Facet</t>
   </si>
   <si>
-    <t>Load;Instrum</t>
-  </si>
-  <si>
     <t>TYPE OF COMPONENT</t>
   </si>
   <si>
@@ -209,9 +203,6 @@
     <t>ℹ️ General</t>
   </si>
   <si>
-    <t>Parent Object</t>
-  </si>
-  <si>
     <t>str</t>
   </si>
   <si>
@@ -240,13 +231,34 @@
   </si>
   <si>
     <t>CodMatExt</t>
+  </si>
+  <si>
+    <t>Views</t>
+  </si>
+  <si>
+    <t>ALL</t>
+  </si>
+  <si>
+    <t>DAMPER, VALVE</t>
+  </si>
+  <si>
+    <t>OtherHvac, Valve</t>
+  </si>
+  <si>
+    <t>Actuator, Sensor</t>
+  </si>
+  <si>
+    <t>Load, Instrum</t>
+  </si>
+  <si>
+    <t>Parent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +275,21 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -300,23 +327,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Accent2" xfId="1" builtinId="33"/>
     <cellStyle name="Accent3" xfId="2" builtinId="37"/>
     <cellStyle name="Accent6" xfId="3" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Texte explicatif" xfId="4" builtinId="53"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -380,18 +410,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{169C0BE5-10BB-4067-85EC-C85BFE5E2020}" name="Table1" displayName="Table1" ref="A1:I18" totalsRowShown="0">
-  <autoFilter ref="A1:I18" xr:uid="{169C0BE5-10BB-4067-85EC-C85BFE5E2020}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{169C0BE5-10BB-4067-85EC-C85BFE5E2020}" name="Table1" displayName="Table1" ref="A1:J18" totalsRowShown="0">
+  <autoFilter ref="A1:J18" xr:uid="{169C0BE5-10BB-4067-85EC-C85BFE5E2020}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J18">
     <sortCondition ref="A1:A18"/>
   </sortState>
-  <tableColumns count="9">
+  <tableColumns count="10">
     <tableColumn id="11" xr3:uid="{F24956A3-9E2B-4F15-AFA3-93301E00FAA9}" name="Order"/>
     <tableColumn id="2" xr3:uid="{7C9D3502-DEAA-4E6A-AD5C-9B9B3E25D96E}" name="Label"/>
-    <tableColumn id="3" xr3:uid="{B003E680-8671-4B35-8B82-FDCA104FEDEE}" name="Facet"/>
-    <tableColumn id="8" xr3:uid="{C4DE5643-8B5D-4C68-8E91-CA3097D11F26}" name="Parent Object"/>
     <tableColumn id="4" xr3:uid="{5F1CC26A-F85C-4D9E-958B-626AAEE5C81E}" name="MUDU"/>
     <tableColumn id="1" xr3:uid="{7800CE7E-FF55-424F-BA36-594534A4A626}" name="Type"/>
+    <tableColumn id="3" xr3:uid="{B003E680-8671-4B35-8B82-FDCA104FEDEE}" name="Facet"/>
+    <tableColumn id="8" xr3:uid="{C4DE5643-8B5D-4C68-8E91-CA3097D11F26}" name="Parent"/>
+    <tableColumn id="6" xr3:uid="{CDD65F4D-3B25-4E90-94E5-98220D75D14F}" name="Views"/>
     <tableColumn id="10" xr3:uid="{EDE825A7-820C-4F6D-87B7-BFFBB3C2DD80}" name="3D Type"/>
     <tableColumn id="5" xr3:uid="{7B9A5008-38A4-40CA-AFBE-A3B688A862E8}" name="2D Type"/>
     <tableColumn id="7" xr3:uid="{BEFD2838-2E43-44CB-87C2-1DEFCFB816D8}" name="1D Type"/>
@@ -694,54 +725,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -749,28 +785,31 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -778,144 +817,159 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
         <v>64</v>
       </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" t="s">
-        <v>56</v>
-      </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -923,28 +977,31 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="E8" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="G8" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -952,28 +1009,31 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="G9" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -981,57 +1041,63 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="H10" t="s">
         <v>16</v>
       </c>
       <c r="I10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
         <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" t="s">
         <v>44</v>
       </c>
-      <c r="F11" t="s">
-        <v>56</v>
-      </c>
       <c r="G11" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="H11" t="s">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="I11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="J11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1039,144 +1105,159 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
         <v>16</v>
       </c>
       <c r="I12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="H13" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="I13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="J13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G14" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="H14" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" t="s">
         <v>14</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>34</v>
       </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" t="s">
-        <v>57</v>
-      </c>
-      <c r="G15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
-      <c r="E16" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1184,53 +1265,59 @@
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="F17" t="s">
         <v>58</v>
       </c>
       <c r="G17" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="H17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" t="s">
         <v>14</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E18" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="G18" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="H18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" t="s">
         <v>14</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1286,20 +1373,20 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1327,34 +1414,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>